<commit_message>
interval reference replaced with table
</commit_message>
<xml_diff>
--- a/tests/eso_files/test_excel_edge_cases.xlsx
+++ b/tests/eso_files/test_excel_edge_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vojtechp1\Desktop\Python\esofile-reader\tests\eso_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2CBA57-7755-475D-B669-B4F0F53A7690}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD65F6AA-D1DC-4927-8397-98FA6460FFAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="2400" windowWidth="21600" windowHeight="11385" tabRatio="907" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1965" windowWidth="21600" windowHeight="11385" tabRatio="907" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blank-lines" sheetId="11" r:id="rId1"/>
@@ -33,9 +33,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="49">
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>interval</t>
   </si>
   <si>
     <t>key</t>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>table2</t>
+  </si>
+  <si>
+    <t>table</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DD09ED-CBB7-4885-A8DE-AB7629744771}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -579,32 +579,32 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -612,10 +612,10 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1">
         <v>11</v>
@@ -1019,255 +1019,255 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895D12D2-F17E-427B-86DF-A2D91DD5A7FC}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,111 +1355,111 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1827,45 +1827,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>4.4459939104838959</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>4.2803046964285896</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>4.0593857443548584</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>4.3944461550000229</v>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>4.4459939104838959</v>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>3.9949510500000178</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>4.4459939104838959</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>4.2526898274193767</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>4.1946986025000204</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>4.4459939104838959</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>4.1946986025000204</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>4.2526898274193767</v>
@@ -2157,45 +2157,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>4.4459939104838959</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>4.2803046964285896</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>4.0593857443548584</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>4.3944461550000229</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>4.4459939104838959</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>3.9949510500000178</v>
@@ -2342,7 +2342,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1">
         <v>10</v>
@@ -2381,88 +2381,88 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2830,30 +2830,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>4.4459939104838959</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>4.2803046964285896</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>4.0593857443548584</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>4.3944461550000229</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>4.4459939104838959</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>3.9949510500000178</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>4.4459939104838959</v>
@@ -3014,7 +3014,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>4.2526898274193767</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>4.1946986025000204</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>4.4459939104838959</v>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>4.1946986025000204</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>4.2526898274193767</v>
@@ -3146,90 +3146,90 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>4.4459939104838959</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>4.2803046964285896</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>4.0593857443548584</v>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>4.3944461550000229</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>4.4459939104838959</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>3.9949510500000178</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>4.4459939104838959</v>
@@ -3390,7 +3390,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>4.2526898274193767</v>
@@ -3413,7 +3413,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>4.1946986025000204</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>4.4459939104838959</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>4.1946986025000204</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>4.2526898274193767</v>
@@ -3514,7 +3514,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3524,111 +3524,111 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3989,7 +3989,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3999,138 +3999,138 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4492,7 +4492,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4502,142 +4502,142 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cover edge test cases, fix failing tests
</commit_message>
<xml_diff>
--- a/tests/eso_files/test_excel_edge_cases.xlsx
+++ b/tests/eso_files/test_excel_edge_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vojtechp1\Desktop\Python\esofile-reader\tests\eso_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD30AB84-1558-4B55-9704-823714BCE8A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D424EED-1D18-4840-8AF7-12605A231056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="615" windowWidth="21600" windowHeight="11385" tabRatio="907" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="907" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blank-lines" sheetId="11" r:id="rId1"/>
@@ -28,14 +28,17 @@
     <sheet name="blank-sheet" sheetId="20" r:id="rId13"/>
     <sheet name="dup-names-table" sheetId="21" r:id="rId14"/>
     <sheet name="dup-names" sheetId="22" r:id="rId15"/>
-    <sheet name="Sheet5" sheetId="23" r:id="rId16"/>
+    <sheet name="simple-monthly" sheetId="24" r:id="rId16"/>
+    <sheet name="test-simple" sheetId="25" r:id="rId17"/>
+    <sheet name="test" sheetId="26" r:id="rId18"/>
+    <sheet name="Sheet5" sheetId="23" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -188,6 +191,9 @@
   </si>
   <si>
     <t>dup-names</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -964,7 +970,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G7" sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2008,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="A1:H7"/>
+      <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FC769F-A0D4-492E-AEE2-3862DCB7B165}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2309,10 +2315,297 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C8055A-C09F-4251-85A2-00B9BEA2040B}">
+  <dimension ref="A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C55440-52E8-41A8-A901-7F5BCE0F6D85}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>19.045026881720428</v>
+      </c>
+      <c r="C5">
+        <v>4.4459939104838959</v>
+      </c>
+      <c r="D5">
+        <v>4.4459939104838959</v>
+      </c>
+      <c r="E5">
+        <v>4.4459939104838959</v>
+      </c>
+      <c r="F5">
+        <v>4.4459939104838959</v>
+      </c>
+      <c r="G5">
+        <v>19.148503481860189</v>
+      </c>
+      <c r="H5">
+        <v>4.8555730384376829E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>32.32626488095238</v>
+      </c>
+      <c r="C6">
+        <v>4.2803046964285896</v>
+      </c>
+      <c r="D6">
+        <v>4.2803046964285896</v>
+      </c>
+      <c r="E6">
+        <v>4.2803046964285896</v>
+      </c>
+      <c r="F6">
+        <v>4.2803046964285896</v>
+      </c>
+      <c r="G6">
+        <v>18.995272108211651</v>
+      </c>
+      <c r="H6">
+        <v>4.8604818741996309E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>62.039650537634408</v>
+      </c>
+      <c r="C7">
+        <v>4.0593857443548584</v>
+      </c>
+      <c r="D7">
+        <v>4.0593857443548584</v>
+      </c>
+      <c r="E7">
+        <v>4.0593857443548584</v>
+      </c>
+      <c r="F7">
+        <v>4.0593857443548584</v>
+      </c>
+      <c r="G7">
+        <v>20.988756152931451</v>
+      </c>
+      <c r="H7">
+        <v>5.4610988883869753E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F70C1AF-3663-4FE0-9806-21313DD9A724}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>365</v>
+      </c>
+      <c r="C5">
+        <v>67.511558219178085</v>
+      </c>
+      <c r="D5">
+        <v>4.2849954413013132</v>
+      </c>
+      <c r="E5">
+        <v>4.2849954413013132</v>
+      </c>
+      <c r="F5">
+        <v>4.2849954413013132</v>
+      </c>
+      <c r="G5">
+        <v>4.2849954413013132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0611307-759F-473C-AA73-D5ABFCE99D45}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>